<commit_message>
update gerber to fix no soldermask for j2 and j3
</commit_message>
<xml_diff>
--- a/03_BOM/NANORACK_LASER.xlsx
+++ b/03_BOM/NANORACK_LASER.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5160"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5160"/>
   </bookViews>
   <sheets>
     <sheet name="NANORACK_LASER" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Samsung Electro-Mechanics</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>0.22uF/25V</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
     <t>DIO-SMD-A</t>
   </si>
   <si>
+    <t>Multicomp</t>
+  </si>
+  <si>
     <t>S2303</t>
   </si>
   <si>
@@ -236,7 +236,7 @@
     <t>Q2, Q4</t>
   </si>
   <si>
-    <t>10K 1%</t>
+    <t>10K/1%</t>
   </si>
   <si>
     <t>ERJ-3EKF1002V</t>
@@ -263,15 +263,24 @@
     <t>300R/0.1%</t>
   </si>
   <si>
+    <t>RT0603BRC07300RL</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
     <t>RES_SMD_0603_SHUNT</t>
   </si>
   <si>
+    <t>Yageo Group</t>
+  </si>
+  <si>
     <t>30K/0.1%</t>
   </si>
   <si>
+    <t>ERA-3AEB303V</t>
+  </si>
+  <si>
     <t>R4, R21</t>
   </si>
   <si>
@@ -305,6 +314,9 @@
     <t>100R/1%</t>
   </si>
   <si>
+    <t>ERJ-PA3D1000V</t>
+  </si>
+  <si>
     <t>R10, R11, R14, R26, R27, R28</t>
   </si>
   <si>
@@ -317,15 +329,24 @@
     <t>20K/0.1%</t>
   </si>
   <si>
+    <t>ERA-3AEB203V</t>
+  </si>
+  <si>
     <t>R16, R30</t>
   </si>
   <si>
     <t>75R/0.1%</t>
   </si>
   <si>
+    <t>TNPW060375R0BEEA</t>
+  </si>
+  <si>
     <t>R20</t>
   </si>
   <si>
+    <t>Vishay</t>
+  </si>
+  <si>
     <t>TPS5430DDAR</t>
   </si>
   <si>
@@ -362,6 +383,9 @@
     <t>INA139</t>
   </si>
   <si>
+    <t>INA139NA/250</t>
+  </si>
+  <si>
     <t>U4, U6</t>
   </si>
   <si>
@@ -371,7 +395,7 @@
     <t>OPA2192</t>
   </si>
   <si>
-    <t>8SOIC</t>
+    <t>OPA2192IDR</t>
   </si>
   <si>
     <t>U5, U7</t>
@@ -392,6 +416,9 @@
     <t>Analog Devices</t>
   </si>
   <si>
+    <t>NOTE</t>
+  </si>
+  <si>
     <t>STATUS</t>
   </si>
   <si>
@@ -399,73 +426,13 @@
   </si>
   <si>
     <t>ORDER</t>
-  </si>
-  <si>
-    <t>Micro Commercial Co</t>
-  </si>
-  <si>
-    <t>SMC Diode Solutions</t>
-  </si>
-  <si>
-    <t>EVVO</t>
-  </si>
-  <si>
-    <t>ERJ-PA3D1000V</t>
-  </si>
-  <si>
-    <t>Custom Socket Laser</t>
-  </si>
-  <si>
-    <t>CONN PIN RCPT .015-.022 SOLDER</t>
-  </si>
-  <si>
-    <t>Mill-Max Manufacturing Corp.</t>
-  </si>
-  <si>
-    <t>0461-1-15-15-21-27-04-0</t>
-  </si>
-  <si>
-    <t>NOTE</t>
-  </si>
-  <si>
-    <t>0510210800</t>
-  </si>
-  <si>
-    <t>CONN RCPT HSG 8POS 1.25MM</t>
-  </si>
-  <si>
-    <t>0500798000</t>
-  </si>
-  <si>
-    <t>CONN SOCKET 26-28AWG CRIMP TIN</t>
-  </si>
-  <si>
-    <t>Mating for J3</t>
-  </si>
-  <si>
-    <t>Cos for mating J3 &amp; J2</t>
-  </si>
-  <si>
-    <t>0510211100</t>
-  </si>
-  <si>
-    <t>CONN RCPT HSG 11POS 1.25MM</t>
-  </si>
-  <si>
-    <t>Mating for J2</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Note:(4 x 36)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -484,10 +451,11 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -495,12 +463,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -535,7 +497,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -558,35 +520,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -595,26 +533,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -895,22 +827,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -936,11 +868,11 @@
       <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>121</v>
+      <c r="H1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -966,19 +898,19 @@
         <v>1</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="6" t="s">
-        <v>122</v>
+      <c r="I2" s="7" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>10</v>
@@ -987,52 +919,52 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="1">
         <v>36</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="7" t="s">
-        <v>122</v>
+      <c r="I3" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1">
         <v>9</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="8" t="s">
-        <v>123</v>
+      <c r="I4" s="7" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>10</v>
@@ -1041,25 +973,25 @@
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1">
         <v>8</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="7" t="s">
-        <v>122</v>
+      <c r="I5" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>10</v>
@@ -1068,25 +1000,25 @@
         <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="1">
         <v>6</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="7" t="s">
-        <v>122</v>
+      <c r="I6" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
@@ -1097,35 +1029,35 @@
         <v>4</v>
       </c>
       <c r="H7" s="1"/>
-      <c r="I7" s="8" t="s">
-        <v>123</v>
+      <c r="I7" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>30</v>
+      <c r="F8" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="7" t="s">
-        <v>122</v>
+      <c r="I8" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1141,18 +1073,14 @@
       <c r="D9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1">
         <v>8</v>
       </c>
       <c r="H9" s="1"/>
-      <c r="I9" s="7" t="s">
-        <v>122</v>
+      <c r="I9" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1168,18 +1096,14 @@
       <c r="D10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
       <c r="G10" s="1">
         <v>24</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="7" t="s">
-        <v>122</v>
+      <c r="I10" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1205,256 +1129,262 @@
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>140</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12" t="s">
+      <c r="I11" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="G12" s="12">
+      <c r="F12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="1">
         <v>1</v>
       </c>
-      <c r="H12" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>122</v>
+      <c r="H12" s="1"/>
+      <c r="I12" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="I13" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="G14" s="12">
+      <c r="I13" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="1">
         <v>1</v>
       </c>
-      <c r="H14" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>136</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="G15" s="12">
-        <v>19</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>122</v>
+      <c r="H14" s="1"/>
+      <c r="I14" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G15" s="1">
+        <v>24</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="G16" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16" s="1"/>
-      <c r="I16" s="7" t="s">
-        <v>122</v>
+      <c r="I16" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="G17" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="7" t="s">
-        <v>122</v>
+      <c r="I17" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="G18" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1"/>
-      <c r="I18" s="7" t="s">
-        <v>122</v>
+      <c r="I18" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="G19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="G20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="8" t="s">
-        <v>123</v>
+      <c r="I20" s="11" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>72</v>
@@ -1463,25 +1393,25 @@
         <v>73</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="G21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H21" s="1"/>
-      <c r="I21" s="7" t="s">
-        <v>122</v>
+      <c r="I21" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>72</v>
@@ -1490,71 +1420,79 @@
         <v>73</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
       </c>
       <c r="H22" s="1"/>
-      <c r="I22" s="7" t="s">
-        <v>122</v>
+      <c r="I22" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>12</v>
+        <v>89</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+        <v>72</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="G23" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="E24" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>92</v>
+      </c>
       <c r="G24" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>72</v>
@@ -1563,24 +1501,25 @@
         <v>73</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>122</v>
+        <v>6</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>72</v>
@@ -1592,22 +1531,22 @@
         <v>86</v>
       </c>
       <c r="G26" s="1">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="7" t="s">
-        <v>122</v>
+      <c r="I26" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>72</v>
@@ -1616,302 +1555,203 @@
         <v>73</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="G27" s="1">
-        <v>12</v>
-      </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="7" t="s">
-        <v>122</v>
+        <v>2</v>
+      </c>
+      <c r="H27" s="9"/>
+      <c r="I27" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>103</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>127</v>
+        <v>80</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="G28" s="1">
-        <v>6</v>
-      </c>
-      <c r="H28" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="H28" s="9"/>
       <c r="I28" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="G29" s="1">
-        <v>8</v>
-      </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="7" t="s">
-        <v>122</v>
+        <v>1</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>110</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>110</v>
+      </c>
       <c r="G30" s="1">
-        <v>2</v>
-      </c>
-      <c r="H30" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="H30" s="9"/>
       <c r="I30" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+        <v>115</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="G31" s="1">
         <v>1</v>
       </c>
-      <c r="H31" s="1"/>
+      <c r="H31" s="10"/>
       <c r="I31" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="G32" s="1">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="7" t="s">
-        <v>122</v>
+        <v>2</v>
+      </c>
+      <c r="H32" s="9"/>
+      <c r="I32" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="G33" s="1">
-        <v>1</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="7" t="s">
-        <v>122</v>
+        <v>2</v>
+      </c>
+      <c r="H33" s="9"/>
+      <c r="I33" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="G34" s="1">
-        <v>1</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1">
-        <v>2</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1">
-        <v>2</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G37" s="1">
         <v>3</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="G38" s="13">
-        <v>144</v>
-      </c>
-      <c r="H38" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="I38" s="7" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F39" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="G39" s="16">
-        <f>SUM(G2:G38)</f>
-        <v>343</v>
+      <c r="H34" s="10"/>
+      <c r="I34" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update step 3d file
</commit_message>
<xml_diff>
--- a/03_BOM/NANORACK_LASER.xlsx
+++ b/03_BOM/NANORACK_LASER.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5160"/>
   </bookViews>
   <sheets>
     <sheet name="NANORACK_LASER" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -110,9 +110,6 @@
     <t>100pF/25V</t>
   </si>
   <si>
-    <t>0603</t>
-  </si>
-  <si>
     <t>C31, C41, C51, C57</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
     <t>ERJ-3EKF4701V</t>
   </si>
   <si>
-    <t>R5</t>
-  </si>
-  <si>
     <t>51R/1%</t>
   </si>
   <si>
@@ -320,12 +314,6 @@
     <t>R10, R11, R14, R26, R27, R28</t>
   </si>
   <si>
-    <t>4.7K 1%</t>
-  </si>
-  <si>
-    <t>R12, R13, R34, R35, R36, R37, R38, R39</t>
-  </si>
-  <si>
     <t>20K/0.1%</t>
   </si>
   <si>
@@ -426,6 +414,66 @@
   </si>
   <si>
     <t>ORDER</t>
+  </si>
+  <si>
+    <t>C0603C101M3HACTU</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>SMC Diode Solutions</t>
+  </si>
+  <si>
+    <t>Micro Commercial Co</t>
+  </si>
+  <si>
+    <t>0510210800</t>
+  </si>
+  <si>
+    <t>CONN RCPT HSG 8POS 1.25MM</t>
+  </si>
+  <si>
+    <t>0500798000</t>
+  </si>
+  <si>
+    <t>CONN SOCKET 26-28AWG CRIMP TIN</t>
+  </si>
+  <si>
+    <t>0510211100</t>
+  </si>
+  <si>
+    <t>CONN RCPT HSG 11POS 1.25MM</t>
+  </si>
+  <si>
+    <t>Mating for J2</t>
+  </si>
+  <si>
+    <t>Mating for J3</t>
+  </si>
+  <si>
+    <t>Cos for mating J2 &amp; J3</t>
+  </si>
+  <si>
+    <t>Custom Socket Laser</t>
+  </si>
+  <si>
+    <t>CONN PIN RCPT .015-.022 SOLDER</t>
+  </si>
+  <si>
+    <t>Mill-Max Manufacturing Corp.</t>
+  </si>
+  <si>
+    <t>0461-1-15-15-21-27-04-0</t>
+  </si>
+  <si>
+    <t>Note:(4 x (24 + 12))</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>R5, R12, R13, R34, R35, R36, R37, R38, R39</t>
   </si>
 </sst>
 </file>
@@ -497,7 +545,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -520,11 +568,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -547,6 +608,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -827,22 +893,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -869,10 +935,10 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -899,7 +965,7 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -926,7 +992,7 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -952,8 +1018,8 @@
         <v>9</v>
       </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="7" t="s">
-        <v>131</v>
+      <c r="I4" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -980,7 +1046,7 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1006,8 +1072,8 @@
         <v>6</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="11" t="s">
-        <v>132</v>
+      <c r="I6" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1015,743 +1081,837 @@
         <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="G7" s="1">
         <v>4</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="1">
         <v>1</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>32</v>
+      </c>
       <c r="G9" s="1">
         <v>8</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="E10" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>35</v>
+      </c>
       <c r="G10" s="1">
         <v>24</v>
       </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="11" t="s">
-        <v>132</v>
+      <c r="I10" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="G11" s="1">
         <v>1</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" s="8" t="s">
-        <v>131</v>
+      <c r="I11" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="1">
+      <c r="A12" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="9">
         <v>1</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="8" t="s">
-        <v>131</v>
+      <c r="H12" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1">
         <v>1</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="1">
+      <c r="A14" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14" s="9">
         <v>1</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="I14" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G15" s="1">
-        <v>24</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="11" t="s">
-        <v>132</v>
+      <c r="A15" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="G15" s="9">
+        <v>19</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G16" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G18" s="1">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="G19" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="8" t="s">
-        <v>131</v>
+      <c r="I19" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="G20" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G21" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="G22" s="1">
         <v>1</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G23" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H23" s="1"/>
-      <c r="I23" s="8" t="s">
-        <v>131</v>
+      <c r="I23" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F24" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="G24" s="1">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H24" s="1"/>
-      <c r="I24" s="8" t="s">
-        <v>131</v>
+      <c r="I24" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F25" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G25" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F26" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="G26" s="1">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F27" s="2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G27" s="1">
-        <v>2</v>
-      </c>
-      <c r="H27" s="9"/>
-      <c r="I27" s="8" t="s">
-        <v>131</v>
+        <v>6</v>
+      </c>
+      <c r="H27" s="1"/>
+      <c r="I27" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="G28" s="1">
-        <v>1</v>
-      </c>
-      <c r="H28" s="9"/>
+        <v>9</v>
+      </c>
+      <c r="H28" s="1"/>
       <c r="I28" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>109</v>
+        <v>72</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="G29" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" s="9"/>
-      <c r="I29" s="8" t="s">
-        <v>131</v>
+      <c r="I29" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>112</v>
+        <v>79</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="G30" s="1">
         <v>1</v>
       </c>
       <c r="H30" s="9"/>
-      <c r="I30" s="8" t="s">
-        <v>131</v>
+      <c r="I30" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
       </c>
-      <c r="H31" s="10"/>
+      <c r="H31" s="9"/>
       <c r="I31" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="G32" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>122</v>
-      </c>
       <c r="G33" s="1">
-        <v>2</v>
-      </c>
-      <c r="H33" s="9"/>
-      <c r="I33" s="8" t="s">
-        <v>131</v>
+        <v>1</v>
+      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="1">
+        <v>2</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G34" s="1">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G35" s="1">
+        <v>2</v>
+      </c>
+      <c r="H35" s="9"/>
+      <c r="I35" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G36" s="1">
         <v>3</v>
       </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="8" t="s">
-        <v>131</v>
+      <c r="H36" s="10"/>
+      <c r="I36" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="10">
+        <v>144</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F38" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="G38" s="1">
+        <f>SUM(G2:G11,G13,G16:G36)</f>
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>